<commit_message>
getStationsByYearRange returns only stations with connections
</commit_message>
<xml_diff>
--- a/data_sheets/TubeMapHistory_DB.xlsx
+++ b/data_sheets/TubeMapHistory_DB.xlsx
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\tubemaphistory\tube-map-history.api\data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B3B249-7011-4F82-9EEA-1A860ABD7941}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C8349-B067-4AE3-B815-82FA817FA37E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="18" r:id="rId1"/>
-    <sheet name="Line_Central Line" sheetId="2" r:id="rId2"/>
-    <sheet name="Line_Jubilee Line" sheetId="3" r:id="rId3"/>
-    <sheet name="Line_Piccadilly Line" sheetId="4" r:id="rId4"/>
-    <sheet name="Line_Victoria Line" sheetId="5" r:id="rId5"/>
-    <sheet name="Line_Bakerloo Line" sheetId="6" r:id="rId6"/>
-    <sheet name="Line_Northern Line" sheetId="7" r:id="rId7"/>
-    <sheet name="Line_District Line" sheetId="8" r:id="rId8"/>
-    <sheet name="Line_Metropolitan Line" sheetId="9" r:id="rId9"/>
-    <sheet name="Line_Circle Line" sheetId="10" r:id="rId10"/>
-    <sheet name="Line_Hammersmith &amp; City Line" sheetId="11" r:id="rId11"/>
-    <sheet name="Line_Waterloo &amp; City Line" sheetId="12" r:id="rId12"/>
-    <sheet name="Line_DLR" sheetId="13" r:id="rId13"/>
+    <sheet name="Line_DLR" sheetId="13" r:id="rId2"/>
+    <sheet name="Line_Central Line" sheetId="2" r:id="rId3"/>
+    <sheet name="Line_Jubilee Line" sheetId="3" r:id="rId4"/>
+    <sheet name="Line_Piccadilly Line" sheetId="4" r:id="rId5"/>
+    <sheet name="Line_Victoria Line" sheetId="5" r:id="rId6"/>
+    <sheet name="Line_Bakerloo Line" sheetId="6" r:id="rId7"/>
+    <sheet name="Line_Northern Line" sheetId="7" r:id="rId8"/>
+    <sheet name="Line_District Line" sheetId="8" r:id="rId9"/>
+    <sheet name="Line_Metropolitan Line" sheetId="9" r:id="rId10"/>
+    <sheet name="Line_Circle Line" sheetId="10" r:id="rId11"/>
+    <sheet name="Line_Hammersmith &amp; City Line" sheetId="11" r:id="rId12"/>
+    <sheet name="Line_Waterloo &amp; City Line" sheetId="12" r:id="rId13"/>
     <sheet name="Line_London Overground" sheetId="14" r:id="rId14"/>
     <sheet name="Line_Elizabeth Line" sheetId="15" r:id="rId15"/>
     <sheet name="Line_Tram" sheetId="16" r:id="rId16"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="673">
   <si>
     <t>name</t>
   </si>
@@ -2433,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B57CB05-6C06-4E09-A4F6-BAF5C3308C96}">
   <dimension ref="A1:E610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="D380" sqref="D380"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4409,6 +4409,9 @@
       <c r="A150" t="s">
         <v>153</v>
       </c>
+      <c r="B150">
+        <v>1987</v>
+      </c>
       <c r="D150">
         <v>-1.7080000000000001E-2</v>
       </c>
@@ -6238,6 +6241,9 @@
       <c r="A298" t="s">
         <v>301</v>
       </c>
+      <c r="B298">
+        <v>2005</v>
+      </c>
       <c r="D298">
         <v>6.2990000000000004E-2</v>
       </c>
@@ -6385,6 +6391,9 @@
       <c r="A310" t="s">
         <v>313</v>
       </c>
+      <c r="B310">
+        <v>2007</v>
+      </c>
       <c r="D310">
         <v>-1.63477E-2</v>
       </c>
@@ -6493,6 +6502,9 @@
       <c r="A319" t="s">
         <v>322</v>
       </c>
+      <c r="B319">
+        <v>1840</v>
+      </c>
       <c r="D319">
         <v>-3.9551099999999999E-2</v>
       </c>
@@ -6532,6 +6544,9 @@
       <c r="A322" t="s">
         <v>325</v>
       </c>
+      <c r="B322">
+        <v>2005</v>
+      </c>
       <c r="D322">
         <v>4.8640000000000003E-2</v>
       </c>
@@ -7472,6 +7487,9 @@
       <c r="A402" t="s">
         <v>405</v>
       </c>
+      <c r="B402">
+        <v>2005</v>
+      </c>
       <c r="D402">
         <v>3.3079999999999998E-2</v>
       </c>
@@ -7483,6 +7501,9 @@
       <c r="A403" t="s">
         <v>406</v>
       </c>
+      <c r="B403">
+        <v>1987</v>
+      </c>
       <c r="D403">
         <v>-1.6503E-2</v>
       </c>
@@ -7956,6 +7977,9 @@
       <c r="A443" t="s">
         <v>446</v>
       </c>
+      <c r="B443">
+        <v>1987</v>
+      </c>
       <c r="D443">
         <v>-5.5480000000000002E-2</v>
       </c>
@@ -8468,6 +8492,9 @@
       <c r="A486" t="s">
         <v>489</v>
       </c>
+      <c r="B486">
+        <v>2011</v>
+      </c>
       <c r="D486">
         <v>1.9913000000000001E-3</v>
       </c>
@@ -8554,6 +8581,9 @@
       <c r="A493" t="s">
         <v>496</v>
       </c>
+      <c r="B493">
+        <v>2011</v>
+      </c>
       <c r="D493">
         <v>-3.2387000000000002E-3</v>
       </c>
@@ -8565,6 +8595,9 @@
       <c r="A494" t="s">
         <v>497</v>
       </c>
+      <c r="B494">
+        <v>2009</v>
+      </c>
       <c r="D494">
         <v>-8.6999999999999994E-3</v>
       </c>
@@ -8951,6 +8984,9 @@
       <c r="A528" t="s">
         <v>531</v>
       </c>
+      <c r="B528">
+        <v>1987</v>
+      </c>
       <c r="D528">
         <v>-7.3466000000000004E-2</v>
       </c>
@@ -9546,6 +9582,9 @@
       <c r="A578" t="s">
         <v>581</v>
       </c>
+      <c r="B578">
+        <v>1987</v>
+      </c>
       <c r="D578">
         <v>-1.9879999999999998E-2</v>
       </c>
@@ -9593,6 +9632,9 @@
       <c r="A582" t="s">
         <v>585</v>
       </c>
+      <c r="B582">
+        <v>2005</v>
+      </c>
       <c r="D582">
         <v>2.2079999999999999E-2</v>
       </c>
@@ -9648,6 +9690,9 @@
       <c r="A587" t="s">
         <v>590</v>
       </c>
+      <c r="B587">
+        <v>1987</v>
+      </c>
       <c r="D587">
         <v>-2.699E-2</v>
       </c>
@@ -9893,6 +9938,9 @@
     <row r="608" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>611</v>
+      </c>
+      <c r="B608">
+        <v>1849</v>
       </c>
       <c r="D608">
         <v>6.7379800000000004E-2</v>
@@ -9929,6 +9977,74 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1" t="s">
+        <v>616</v>
+      </c>
+      <c r="E1" t="s">
+        <v>617</v>
+      </c>
+      <c r="F1" t="s">
+        <v>618</v>
+      </c>
+      <c r="G1" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1" t="s">
+        <v>620</v>
+      </c>
+      <c r="I1" t="s">
+        <v>621</v>
+      </c>
+      <c r="J1" t="s">
+        <v>622</v>
+      </c>
+      <c r="K1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>647</v>
+      </c>
+      <c r="C2" t="s">
+        <v>648</v>
+      </c>
+      <c r="D2" t="s">
+        <v>649</v>
+      </c>
+      <c r="E2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:K2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -9996,7 +10112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -10096,7 +10212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -10192,138 +10308,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:K4" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>614</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>615</v>
-      </c>
-      <c r="D1" t="s">
-        <v>616</v>
-      </c>
-      <c r="E1" t="s">
-        <v>617</v>
-      </c>
-      <c r="F1" t="s">
-        <v>618</v>
-      </c>
-      <c r="G1" t="s">
-        <v>619</v>
-      </c>
-      <c r="H1" t="s">
-        <v>620</v>
-      </c>
-      <c r="I1" t="s">
-        <v>621</v>
-      </c>
-      <c r="J1" t="s">
-        <v>622</v>
-      </c>
-      <c r="K1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>659</v>
-      </c>
-      <c r="C2" t="s">
-        <v>660</v>
-      </c>
-      <c r="D2" t="s">
-        <v>661</v>
-      </c>
-      <c r="E2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>619</v>
-      </c>
-      <c r="B4" t="s">
-        <v>619</v>
-      </c>
-      <c r="C4" t="s">
-        <v>619</v>
-      </c>
-      <c r="D4" t="s">
-        <v>619</v>
-      </c>
-      <c r="E4" t="s">
-        <v>619</v>
-      </c>
-      <c r="F4" t="s">
-        <v>619</v>
-      </c>
-      <c r="G4" t="s">
-        <v>619</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" t="s">
-        <v>437</v>
-      </c>
-      <c r="J4">
-        <v>1994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>619</v>
-      </c>
-      <c r="B5" t="s">
-        <v>619</v>
-      </c>
-      <c r="C5" t="s">
-        <v>619</v>
-      </c>
-      <c r="D5" t="s">
-        <v>619</v>
-      </c>
-      <c r="E5" t="s">
-        <v>619</v>
-      </c>
-      <c r="F5" t="s">
-        <v>619</v>
-      </c>
-      <c r="G5" t="s">
-        <v>619</v>
-      </c>
-      <c r="H5" t="s">
-        <v>437</v>
-      </c>
-      <c r="I5" t="s">
-        <v>140</v>
-      </c>
-      <c r="J5">
-        <v>1994</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:K5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -10601,6 +10585,492 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:K47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1" t="s">
+        <v>616</v>
+      </c>
+      <c r="E1" t="s">
+        <v>617</v>
+      </c>
+      <c r="F1" t="s">
+        <v>618</v>
+      </c>
+      <c r="G1" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1" t="s">
+        <v>620</v>
+      </c>
+      <c r="I1" t="s">
+        <v>621</v>
+      </c>
+      <c r="J1" t="s">
+        <v>622</v>
+      </c>
+      <c r="K1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>659</v>
+      </c>
+      <c r="C2" t="s">
+        <v>660</v>
+      </c>
+      <c r="D2" t="s">
+        <v>661</v>
+      </c>
+      <c r="E2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>619</v>
+      </c>
+      <c r="B4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C4" t="s">
+        <v>619</v>
+      </c>
+      <c r="D4" t="s">
+        <v>619</v>
+      </c>
+      <c r="E4" t="s">
+        <v>619</v>
+      </c>
+      <c r="F4" t="s">
+        <v>619</v>
+      </c>
+      <c r="G4" t="s">
+        <v>619</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>446</v>
+      </c>
+      <c r="J4">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>619</v>
+      </c>
+      <c r="B5" t="s">
+        <v>619</v>
+      </c>
+      <c r="C5" t="s">
+        <v>619</v>
+      </c>
+      <c r="D5" t="s">
+        <v>619</v>
+      </c>
+      <c r="E5" t="s">
+        <v>619</v>
+      </c>
+      <c r="F5" t="s">
+        <v>619</v>
+      </c>
+      <c r="G5" t="s">
+        <v>619</v>
+      </c>
+      <c r="H5" t="s">
+        <v>531</v>
+      </c>
+      <c r="I5" t="s">
+        <v>446</v>
+      </c>
+      <c r="J5">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>322</v>
+      </c>
+      <c r="J6">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>590</v>
+      </c>
+      <c r="J7">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>406</v>
+      </c>
+      <c r="J8">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>437</v>
+      </c>
+      <c r="J12">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>408</v>
+      </c>
+      <c r="J14">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>435</v>
+      </c>
+      <c r="J15">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>142</v>
+      </c>
+      <c r="J17">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>206</v>
+      </c>
+      <c r="J18">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" t="s">
+        <v>585</v>
+      </c>
+      <c r="J20">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>405</v>
+      </c>
+      <c r="J21">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>325</v>
+      </c>
+      <c r="J22">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>301</v>
+      </c>
+      <c r="J23">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="24" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>611</v>
+      </c>
+      <c r="J24">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>590</v>
+      </c>
+      <c r="I25" t="s">
+        <v>581</v>
+      </c>
+      <c r="J25">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>86</v>
+      </c>
+      <c r="J26">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>467</v>
+      </c>
+      <c r="J27">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="28" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J28">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="29" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>353</v>
+      </c>
+      <c r="J29">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="30" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>284</v>
+      </c>
+      <c r="J30">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="31" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>141</v>
+      </c>
+      <c r="J31">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="32" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>223</v>
+      </c>
+      <c r="J32">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J33">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>179</v>
+      </c>
+      <c r="J34">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I35" t="s">
+        <v>317</v>
+      </c>
+      <c r="J35">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>406</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="37" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>313</v>
+      </c>
+      <c r="J37">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="38" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>153</v>
+      </c>
+      <c r="J38">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="39" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J39">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="40" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>409</v>
+      </c>
+      <c r="J40">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="41" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>495</v>
+      </c>
+      <c r="J41">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="42" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I42" t="s">
+        <v>489</v>
+      </c>
+      <c r="J42">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="43" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>577</v>
+      </c>
+      <c r="J43">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="44" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="45" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>496</v>
+      </c>
+      <c r="J45">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="46" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>495</v>
+      </c>
+      <c r="J46">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="47" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>497</v>
+      </c>
+      <c r="J47">
+        <v>1994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:K3 A5:G5 A4:G4 J4:K4 J5:K5" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
@@ -12151,7 +12621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -12435,11 +12905,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -12714,7 +13184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
@@ -12912,11 +13382,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -13182,7 +13652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -13314,7 +13784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -13412,72 +13882,4 @@
     <ignoredError sqref="A1:K4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>614</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>615</v>
-      </c>
-      <c r="D1" t="s">
-        <v>616</v>
-      </c>
-      <c r="E1" t="s">
-        <v>617</v>
-      </c>
-      <c r="F1" t="s">
-        <v>618</v>
-      </c>
-      <c r="G1" t="s">
-        <v>619</v>
-      </c>
-      <c r="H1" t="s">
-        <v>620</v>
-      </c>
-      <c r="I1" t="s">
-        <v>621</v>
-      </c>
-      <c r="J1" t="s">
-        <v>622</v>
-      </c>
-      <c r="K1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>647</v>
-      </c>
-      <c r="C2" t="s">
-        <v>648</v>
-      </c>
-      <c r="D2" t="s">
-        <v>649</v>
-      </c>
-      <c r="E2" t="s">
-        <v>627</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:K2" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>